<commit_message>
Problem 2 Homework 5
Problem 2 for homework 5 seems to be finished, I might have to make some slight adjustments to the code and re-run to get a more accurate result.
</commit_message>
<xml_diff>
--- a/hw5/Statistics.xlsx
+++ b/hw5/Statistics.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem1" sheetId="1" r:id="rId1"/>
+    <sheet name="Problem2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Benchmark</t>
   </si>
@@ -36,6 +37,24 @@
   </si>
   <si>
     <t>Total Instructions Executed</t>
+  </si>
+  <si>
+    <t>Basic Blocks</t>
+  </si>
+  <si>
+    <t>Memory Reads</t>
+  </si>
+  <si>
+    <t>Memory Writes</t>
+  </si>
+  <si>
+    <t>Total Instructions</t>
+  </si>
+  <si>
+    <t>mm_mult_serial 256x256</t>
+  </si>
+  <si>
+    <t>accumulate array 1x256</t>
   </si>
 </sst>
 </file>
@@ -413,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C27888C-8B82-438A-92A4-E579728B9758}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,4 +469,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B57EFD-2F6B-409F-A34F-0C2118B5BCC1}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2431</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3816</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2559</v>
+      </c>
+      <c r="E2" s="3">
+        <v>482639275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3429</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5634</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4632</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1421207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>61000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>260281</v>
+      </c>
+      <c r="D4" s="3">
+        <v>251764</v>
+      </c>
+      <c r="E4" s="3">
+        <v>583459817248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>23105</v>
+      </c>
+      <c r="C5" s="3">
+        <v>53870</v>
+      </c>
+      <c r="D5" s="3">
+        <v>39434</v>
+      </c>
+      <c r="E5" s="3">
+        <v>257156226792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the source code for problem 2 to use what I think is the correct trace options to get the basic block count.
</commit_message>
<xml_diff>
--- a/hw5/Statistics.xlsx
+++ b/hw5/Statistics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UAH\CPE_631_Advanced_Computer_Architecture\CPE_631_Advanced_Computer_Architecture\hw5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krray\OneDrive\Documents\GitHub\CPE_631_Advanced_Computer_Architecture\hw5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" activeTab="1" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem1" sheetId="1" r:id="rId1"/>
@@ -61,10 +61,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,11 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,12 +444,12 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +465,7 @@
         <v>583459817340</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -476,19 +484,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,12 +513,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <v>2431</v>
+        <v>3104</v>
       </c>
       <c r="C2" s="3">
         <v>3816</v>
@@ -519,15 +527,15 @@
         <v>2559</v>
       </c>
       <c r="E2" s="3">
-        <v>482639275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>482639296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <v>3429</v>
+        <v>4619</v>
       </c>
       <c r="C3" s="3">
         <v>5634</v>
@@ -536,41 +544,41 @@
         <v>4632</v>
       </c>
       <c r="E3" s="3">
-        <v>1421207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1421192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
-        <v>61000</v>
+        <v>104862</v>
       </c>
       <c r="C4" s="3">
-        <v>260281</v>
+        <v>260269</v>
       </c>
       <c r="D4" s="3">
-        <v>251764</v>
+        <v>251753</v>
       </c>
       <c r="E4" s="3">
-        <v>583459817248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+        <v>583459817334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <v>23105</v>
-      </c>
-      <c r="C5" s="3">
-        <v>53870</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B5" s="5">
+        <v>37987</v>
+      </c>
+      <c r="C5" s="5">
+        <v>53881</v>
+      </c>
+      <c r="D5" s="5">
         <v>39434</v>
       </c>
-      <c r="E5" s="3">
-        <v>257156226792</v>
+      <c r="E5" s="5">
+        <v>257156226729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the updates for problem 2 and some extra code that is good to have around. Also, updated the statistics to have some information from testing problem 2.
</commit_message>
<xml_diff>
--- a/hw5/Statistics.xlsx
+++ b/hw5/Statistics.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" activeTab="1" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" activeTab="2" xr2:uid="{5D65992B-3718-47DC-BCCC-F32955465A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem1" sheetId="1" r:id="rId1"/>
     <sheet name="Problem2" sheetId="2" r:id="rId2"/>
+    <sheet name="Problem2Bonus" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>Benchmark</t>
   </si>
@@ -55,6 +56,213 @@
   </si>
   <si>
     <t>accumulate array 1x256</t>
+  </si>
+  <si>
+    <t>time=150.98047800 seconds</t>
+  </si>
+  <si>
+    <t>Memory Reads[2] = 121870480</t>
+  </si>
+  <si>
+    <t>Memory Writes[2] = 11695138</t>
+  </si>
+  <si>
+    <t>Basic Blocks[2] = 7594768</t>
+  </si>
+  <si>
+    <t>Total Instructions[2] = 197563103</t>
+  </si>
+  <si>
+    <t>Memory Reads[1] = 121545494</t>
+  </si>
+  <si>
+    <t>Memory Writes[1] = 11695306</t>
+  </si>
+  <si>
+    <t>Basic Blocks[1] = 6944212</t>
+  </si>
+  <si>
+    <t>Total Instructions[1] = 195611910</t>
+  </si>
+  <si>
+    <t>Memory Reads[3] = 121854939</t>
+  </si>
+  <si>
+    <t>Memory Writes[3] = 11694888</t>
+  </si>
+  <si>
+    <t>Basic Blocks[3] = 7564592</t>
+  </si>
+  <si>
+    <t>Total Instructions[3] = 197471670</t>
+  </si>
+  <si>
+    <t>Memory Reads[0] = 125361231</t>
+  </si>
+  <si>
+    <t>Memory Writes[0] = 13353706</t>
+  </si>
+  <si>
+    <t>Basic Blocks[0] = 9019806</t>
+  </si>
+  <si>
+    <t>Total Instructions[0] = 209355661</t>
+  </si>
+  <si>
+    <t>Total number of threads = 4</t>
+  </si>
+  <si>
+    <t>time=0.16943400 seconds</t>
+  </si>
+  <si>
+    <t>Memory Reads[3] = 68104</t>
+  </si>
+  <si>
+    <t>Memory Writes[3] = 1528</t>
+  </si>
+  <si>
+    <t>Basic Blocks[3] = 133237</t>
+  </si>
+  <si>
+    <t>Total Instructions[3] = 403338</t>
+  </si>
+  <si>
+    <t>Memory Reads[2] = 123182</t>
+  </si>
+  <si>
+    <t>Memory Writes[2] = 1521</t>
+  </si>
+  <si>
+    <t>Basic Blocks[2] = 243396</t>
+  </si>
+  <si>
+    <t>Total Instructions[2] = 733805</t>
+  </si>
+  <si>
+    <t>Memory Reads[1] = 128701</t>
+  </si>
+  <si>
+    <t>Memory Writes[1] = 1804</t>
+  </si>
+  <si>
+    <t>Basic Blocks[1] = 253410</t>
+  </si>
+  <si>
+    <t>Total Instructions[1] = 764766</t>
+  </si>
+  <si>
+    <t>Memory Reads[0] = 349752</t>
+  </si>
+  <si>
+    <t>Memory Writes[0] = 119591</t>
+  </si>
+  <si>
+    <t>Basic Blocks[0] = 252405</t>
+  </si>
+  <si>
+    <t>Total Instructions[0] = 1449429</t>
+  </si>
+  <si>
+    <t>time=143.96135900 seconds</t>
+  </si>
+  <si>
+    <t>Memory Reads[2] = 121907204</t>
+  </si>
+  <si>
+    <t>Memory Writes[2] = 11695170</t>
+  </si>
+  <si>
+    <t>Basic Blocks[2] = 7668105</t>
+  </si>
+  <si>
+    <t>Total Instructions[2] = 197783103</t>
+  </si>
+  <si>
+    <t>Memory Reads[3] = 121851383</t>
+  </si>
+  <si>
+    <t>Memory Writes[3] = 11695014</t>
+  </si>
+  <si>
+    <t>Basic Blocks[3] = 7557022</t>
+  </si>
+  <si>
+    <t>Total Instructions[3] = 197449416</t>
+  </si>
+  <si>
+    <t>Memory Reads[1] = 121595688</t>
+  </si>
+  <si>
+    <t>Memory Writes[1] = 11695305</t>
+  </si>
+  <si>
+    <t>Basic Blocks[1] = 7044600</t>
+  </si>
+  <si>
+    <t>Total Instructions[1] = 195913074</t>
+  </si>
+  <si>
+    <t>Memory Reads[0] = 125361271</t>
+  </si>
+  <si>
+    <t>Memory Writes[0] = 13353728</t>
+  </si>
+  <si>
+    <t>Basic Blocks[0] = 9019230</t>
+  </si>
+  <si>
+    <t>Total Instructions[0] = 209354000</t>
+  </si>
+  <si>
+    <t>time=0.17670500 seconds</t>
+  </si>
+  <si>
+    <t>Memory Reads[1] = 136010</t>
+  </si>
+  <si>
+    <t>Memory Writes[1] = 1808</t>
+  </si>
+  <si>
+    <t>Basic Blocks[1] = 268022</t>
+  </si>
+  <si>
+    <t>Total Instructions[1] = 808608</t>
+  </si>
+  <si>
+    <t>Memory Reads[2] = 122385</t>
+  </si>
+  <si>
+    <t>Memory Writes[2] = 1648</t>
+  </si>
+  <si>
+    <t>Basic Blocks[2] = 241347</t>
+  </si>
+  <si>
+    <t>Total Instructions[2] = 728118</t>
+  </si>
+  <si>
+    <t>Memory Reads[3] = 82365</t>
+  </si>
+  <si>
+    <t>Memory Writes[3] = 1639</t>
+  </si>
+  <si>
+    <t>Basic Blocks[3] = 161317</t>
+  </si>
+  <si>
+    <t>Total Instructions[3] = 488016</t>
+  </si>
+  <si>
+    <t>Memory Reads[0] = 348213</t>
+  </si>
+  <si>
+    <t>Memory Writes[0] = 119347</t>
+  </si>
+  <si>
+    <t>Basic Blocks[0] = 249596</t>
+  </si>
+  <si>
+    <t>Total Instructions[0] = 1440102</t>
   </si>
 </sst>
 </file>
@@ -483,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B57EFD-2F6B-409F-A34F-0C2118B5BCC1}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,4 +793,271 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CC488F-CD96-429A-A782-0F89AEC6722F}">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>